<commit_message>
Final Clean and Merge
</commit_message>
<xml_diff>
--- a/merged_data/independent_sg.xlsx
+++ b/merged_data/independent_sg.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="310">
   <si>
     <t>headline</t>
   </si>
@@ -3233,6 +3233,9 @@
       <c r="D96" t="s">
         <v>301</v>
       </c>
+      <c r="E96" t="s">
+        <v>308</v>
+      </c>
       <c r="F96" t="s">
         <v>309</v>
       </c>
@@ -3270,6 +3273,9 @@
       <c r="D98" t="s">
         <v>301</v>
       </c>
+      <c r="E98" t="s">
+        <v>308</v>
+      </c>
       <c r="F98" t="s">
         <v>309</v>
       </c>
@@ -3287,6 +3293,9 @@
       <c r="D99" t="s">
         <v>301</v>
       </c>
+      <c r="E99" t="s">
+        <v>308</v>
+      </c>
       <c r="F99" t="s">
         <v>309</v>
       </c>
@@ -3304,6 +3313,9 @@
       <c r="D100" t="s">
         <v>301</v>
       </c>
+      <c r="E100" t="s">
+        <v>308</v>
+      </c>
       <c r="F100" t="s">
         <v>309</v>
       </c>
@@ -3321,6 +3333,9 @@
       <c r="D101" t="s">
         <v>301</v>
       </c>
+      <c r="E101" t="s">
+        <v>308</v>
+      </c>
       <c r="F101" t="s">
         <v>309</v>
       </c>
@@ -3338,6 +3353,9 @@
       <c r="D102" t="s">
         <v>301</v>
       </c>
+      <c r="E102" t="s">
+        <v>308</v>
+      </c>
       <c r="F102" t="s">
         <v>309</v>
       </c>
@@ -3355,6 +3373,9 @@
       <c r="D103" t="s">
         <v>301</v>
       </c>
+      <c r="E103" t="s">
+        <v>308</v>
+      </c>
       <c r="F103" t="s">
         <v>309</v>
       </c>
@@ -3371,6 +3392,9 @@
       </c>
       <c r="D104" t="s">
         <v>301</v>
+      </c>
+      <c r="E104" t="s">
+        <v>308</v>
       </c>
       <c r="F104" t="s">
         <v>309</v>

</xml_diff>